<commit_message>
abs error fig 그리기
</commit_message>
<xml_diff>
--- a/estimation/VAEwithDG/DG_DenseRegressor_1st_torch/vaelstm_3rd_torch/IWALQQ_AE_1st/angle/60/0_fold/0.xlsx
+++ b/estimation/VAEwithDG/DG_DenseRegressor_1st_torch/vaelstm_3rd_torch/IWALQQ_AE_1st/angle/60/0_fold/0.xlsx
@@ -479,13 +479,13 @@
         <v>-12.84196021680824</v>
       </c>
       <c r="E2" t="n">
-        <v>-21.58960023064327</v>
+        <v>-21.59712441221145</v>
       </c>
       <c r="F2" t="n">
-        <v>-0.07020627331283415</v>
+        <v>-0.07101784845274203</v>
       </c>
       <c r="G2" t="n">
-        <v>-8.924192820288939</v>
+        <v>-8.919890494246053</v>
       </c>
     </row>
     <row r="3">
@@ -502,13 +502,13 @@
         <v>-12.71643442446967</v>
       </c>
       <c r="E3" t="n">
-        <v>-21.73659311110393</v>
+        <v>-21.74423462883692</v>
       </c>
       <c r="F3" t="n">
-        <v>-0.2025908012551571</v>
+        <v>-0.2036028256766085</v>
       </c>
       <c r="G3" t="n">
-        <v>-8.436137931785419</v>
+        <v>-8.432392952525364</v>
       </c>
     </row>
     <row r="4">
@@ -525,13 +525,13 @@
         <v>-12.47310014886157</v>
       </c>
       <c r="E4" t="n">
-        <v>-21.91859128073171</v>
+        <v>-21.92526966411191</v>
       </c>
       <c r="F4" t="n">
-        <v>-0.3597919280539403</v>
+        <v>-0.3608235085028594</v>
       </c>
       <c r="G4" t="n">
-        <v>-8.33064294161113</v>
+        <v>-8.327069077591414</v>
       </c>
     </row>
     <row r="5">
@@ -548,13 +548,13 @@
         <v>-12.11331913943963</v>
       </c>
       <c r="E5" t="n">
-        <v>-22.03768259900289</v>
+        <v>-22.04397963984747</v>
       </c>
       <c r="F5" t="n">
-        <v>-0.3865885746915012</v>
+        <v>-0.3872925916803369</v>
       </c>
       <c r="G5" t="n">
-        <v>-7.804204460195462</v>
+        <v>-7.800821267443556</v>
       </c>
     </row>
     <row r="6">
@@ -571,13 +571,13 @@
         <v>-11.64090941610433</v>
       </c>
       <c r="E6" t="n">
-        <v>-21.97076676201542</v>
+        <v>-21.97574866001281</v>
       </c>
       <c r="F6" t="n">
-        <v>-0.509092419755789</v>
+        <v>-0.5096986566072865</v>
       </c>
       <c r="G6" t="n">
-        <v>-7.111119290714131</v>
+        <v>-7.107662762859221</v>
       </c>
     </row>
     <row r="7">
@@ -594,13 +594,13 @@
         <v>-11.07914292675722</v>
       </c>
       <c r="E7" t="n">
-        <v>-22.24107506268028</v>
+        <v>-22.24587117841673</v>
       </c>
       <c r="F7" t="n">
-        <v>-0.657175548747776</v>
+        <v>-0.6582315742310295</v>
       </c>
       <c r="G7" t="n">
-        <v>-6.521861960065473</v>
+        <v>-6.518708550636313</v>
       </c>
     </row>
     <row r="8">
@@ -617,13 +617,13 @@
         <v>-10.44983419553826</v>
       </c>
       <c r="E8" t="n">
-        <v>-22.6279079530112</v>
+        <v>-22.63287029498111</v>
       </c>
       <c r="F8" t="n">
-        <v>-0.8262618512400294</v>
+        <v>-0.827488991963625</v>
       </c>
       <c r="G8" t="n">
-        <v>-6.101001581940833</v>
+        <v>-6.098596190562311</v>
       </c>
     </row>
     <row r="9">
@@ -640,13 +640,13 @@
         <v>-9.763522020068496</v>
       </c>
       <c r="E9" t="n">
-        <v>-22.89911583093957</v>
+        <v>-22.90411239595755</v>
       </c>
       <c r="F9" t="n">
-        <v>-0.9537035932399013</v>
+        <v>-0.9547840637574896</v>
       </c>
       <c r="G9" t="n">
-        <v>-5.776718645465231</v>
+        <v>-5.774151916860101</v>
       </c>
     </row>
     <row r="10">
@@ -663,13 +663,13 @@
         <v>-9.032633399222505</v>
       </c>
       <c r="E10" t="n">
-        <v>-23.34685107981164</v>
+        <v>-23.35176453171289</v>
       </c>
       <c r="F10" t="n">
-        <v>-1.052745094349864</v>
+        <v>-1.053933123018525</v>
       </c>
       <c r="G10" t="n">
-        <v>-5.47357577468217</v>
+        <v>-5.471898845326819</v>
       </c>
     </row>
     <row r="11">
@@ -686,13 +686,13 @@
         <v>-8.275057976045334</v>
       </c>
       <c r="E11" t="n">
-        <v>-23.76073973414406</v>
+        <v>-23.76532562258522</v>
       </c>
       <c r="F11" t="n">
-        <v>-1.313969620255997</v>
+        <v>-1.31515275991779</v>
       </c>
       <c r="G11" t="n">
-        <v>-5.083354802592487</v>
+        <v>-5.080851631076627</v>
       </c>
     </row>
     <row r="12">
@@ -709,13 +709,13 @@
         <v>-7.495862978727758</v>
       </c>
       <c r="E12" t="n">
-        <v>-24.22675986869839</v>
+        <v>-24.23131153409149</v>
       </c>
       <c r="F12" t="n">
-        <v>-1.234440145551891</v>
+        <v>-1.235178385588796</v>
       </c>
       <c r="G12" t="n">
-        <v>-4.92254558872592</v>
+        <v>-4.920345535635809</v>
       </c>
     </row>
     <row r="13">
@@ -732,13 +732,13 @@
         <v>-6.693916057904498</v>
       </c>
       <c r="E13" t="n">
-        <v>-24.81347491577625</v>
+        <v>-24.81827592051956</v>
       </c>
       <c r="F13" t="n">
-        <v>-1.164752241670886</v>
+        <v>-1.16582293417474</v>
       </c>
       <c r="G13" t="n">
-        <v>-4.846932208522214</v>
+        <v>-4.845005939816649</v>
       </c>
     </row>
     <row r="14">
@@ -755,13 +755,13 @@
         <v>-5.886001349666778</v>
       </c>
       <c r="E14" t="n">
-        <v>-25.41478364835186</v>
+        <v>-25.41933042473809</v>
       </c>
       <c r="F14" t="n">
-        <v>-1.098178635164105</v>
+        <v>-1.099131991503153</v>
       </c>
       <c r="G14" t="n">
-        <v>-4.717275746411629</v>
+        <v>-4.714933912122377</v>
       </c>
     </row>
     <row r="15">
@@ -778,13 +778,13 @@
         <v>-5.076858783042173</v>
       </c>
       <c r="E15" t="n">
-        <v>-26.02895046898745</v>
+        <v>-26.03384925386809</v>
       </c>
       <c r="F15" t="n">
-        <v>-1.054857145316372</v>
+        <v>-1.055947393847694</v>
       </c>
       <c r="G15" t="n">
-        <v>-4.734269934281025</v>
+        <v>-4.732485446774602</v>
       </c>
     </row>
     <row r="16">
@@ -801,13 +801,13 @@
         <v>-4.269265041209697</v>
       </c>
       <c r="E16" t="n">
-        <v>-26.80078287207418</v>
+        <v>-26.80631967235096</v>
       </c>
       <c r="F16" t="n">
-        <v>-0.9616140063505697</v>
+        <v>-0.9623082453256716</v>
       </c>
       <c r="G16" t="n">
-        <v>-4.686284331882256</v>
+        <v>-4.684421620265961</v>
       </c>
     </row>
     <row r="17">
@@ -824,13 +824,13 @@
         <v>-3.479964770861571</v>
       </c>
       <c r="E17" t="n">
-        <v>-27.56017275268461</v>
+        <v>-27.56506175955152</v>
       </c>
       <c r="F17" t="n">
-        <v>-0.8382594740914386</v>
+        <v>-0.8389732690940083</v>
       </c>
       <c r="G17" t="n">
-        <v>-4.715256586575594</v>
+        <v>-4.713750772460584</v>
       </c>
     </row>
     <row r="18">
@@ -847,13 +847,13 @@
         <v>-2.72093704491223</v>
       </c>
       <c r="E18" t="n">
-        <v>-28.44206647835933</v>
+        <v>-28.44724882563825</v>
       </c>
       <c r="F18" t="n">
-        <v>-0.6708403229408032</v>
+        <v>-0.6711629973940195</v>
       </c>
       <c r="G18" t="n">
-        <v>-4.968707591563331</v>
+        <v>-4.968101354711834</v>
       </c>
     </row>
     <row r="19">
@@ -870,13 +870,13 @@
         <v>-2.001365747441985</v>
       </c>
       <c r="E19" t="n">
-        <v>-29.09366598007145</v>
+        <v>-29.09880188178515</v>
       </c>
       <c r="F19" t="n">
-        <v>-0.4186213476835279</v>
+        <v>-0.4190662473084172</v>
       </c>
       <c r="G19" t="n">
-        <v>-5.258322580345639</v>
+        <v>-5.258454583531045</v>
       </c>
     </row>
     <row r="20">
@@ -893,13 +893,13 @@
         <v>-1.335721915267746</v>
       </c>
       <c r="E20" t="n">
-        <v>-29.51664329816946</v>
+        <v>-29.52153474953981</v>
       </c>
       <c r="F20" t="n">
-        <v>-0.2146324251683686</v>
+        <v>-0.2151115478413263</v>
       </c>
       <c r="G20" t="n">
-        <v>-5.582840189150852</v>
+        <v>-5.582297509388625</v>
       </c>
     </row>
     <row r="21">
@@ -916,13 +916,13 @@
         <v>-0.7372717129417354</v>
       </c>
       <c r="E21" t="n">
-        <v>-30.11163054486614</v>
+        <v>-30.11647555067126</v>
       </c>
       <c r="F21" t="n">
-        <v>0.1970855101151399</v>
+        <v>0.1968948388473302</v>
       </c>
       <c r="G21" t="n">
-        <v>-5.910613876529431</v>
+        <v>-5.909464959915706</v>
       </c>
     </row>
     <row r="22">
@@ -939,13 +939,13 @@
         <v>-0.2117656691844328</v>
       </c>
       <c r="E22" t="n">
-        <v>-30.66655971379876</v>
+        <v>-30.67202317897254</v>
       </c>
       <c r="F22" t="n">
-        <v>0.2531526408649205</v>
+        <v>0.2529668586039778</v>
       </c>
       <c r="G22" t="n">
-        <v>-6.179665702429495</v>
+        <v>-6.179098577632932</v>
       </c>
     </row>
     <row r="23">
@@ -962,13 +962,13 @@
         <v>0.2377845783657954</v>
       </c>
       <c r="E23" t="n">
-        <v>-30.9929424787237</v>
+        <v>-30.99837660985628</v>
       </c>
       <c r="F23" t="n">
-        <v>0.5378835117871802</v>
+        <v>0.5376097274026329</v>
       </c>
       <c r="G23" t="n">
-        <v>-6.476232858976555</v>
+        <v>-6.475215945548237</v>
       </c>
     </row>
     <row r="24">
@@ -985,13 +985,13 @@
         <v>0.6076276132382513</v>
       </c>
       <c r="E24" t="n">
-        <v>-31.19806809533542</v>
+        <v>-31.20423068849117</v>
       </c>
       <c r="F24" t="n">
-        <v>0.7304077131994239</v>
+        <v>0.7301730408698121</v>
       </c>
       <c r="G24" t="n">
-        <v>-6.737848505432041</v>
+        <v>-6.737247157587411</v>
       </c>
     </row>
     <row r="25">
@@ -1008,13 +1008,13 @@
         <v>0.9024407677695052</v>
       </c>
       <c r="E25" t="n">
-        <v>-31.49685486100006</v>
+        <v>-31.50327412701632</v>
       </c>
       <c r="F25" t="n">
-        <v>0.9687174639203262</v>
+        <v>0.9687223529271931</v>
       </c>
       <c r="G25" t="n">
-        <v>-6.793607628749206</v>
+        <v>-6.792673828437626</v>
       </c>
     </row>
     <row r="26">
@@ -1031,13 +1031,13 @@
         <v>1.130750603553289</v>
       </c>
       <c r="E26" t="n">
-        <v>-31.40931963755138</v>
+        <v>-31.41541134010756</v>
       </c>
       <c r="F26" t="n">
-        <v>0.9992688678316777</v>
+        <v>0.9988973033097921</v>
       </c>
       <c r="G26" t="n">
-        <v>-6.976549376702296</v>
+        <v>-6.976358705434487</v>
       </c>
     </row>
     <row r="27">
@@ -1054,13 +1054,13 @@
         <v>1.296728828350363</v>
       </c>
       <c r="E27" t="n">
-        <v>-31.50882314981027</v>
+        <v>-31.51519352575786</v>
       </c>
       <c r="F27" t="n">
-        <v>1.245181024230633</v>
+        <v>1.244941462894154</v>
       </c>
       <c r="G27" t="n">
-        <v>-7.234918722598151</v>
+        <v>-7.235045836776691</v>
       </c>
     </row>
     <row r="28">
@@ -1077,13 +1077,13 @@
         <v>1.409879374076194</v>
       </c>
       <c r="E28" t="n">
-        <v>-31.32806923243012</v>
+        <v>-31.33475494932063</v>
       </c>
       <c r="F28" t="n">
-        <v>1.40370707189035</v>
+        <v>1.403902632165027</v>
       </c>
       <c r="G28" t="n">
-        <v>-7.417811580482572</v>
+        <v>-7.418012029764116</v>
       </c>
     </row>
     <row r="29">
@@ -1100,13 +1100,13 @@
         <v>1.479280467169328</v>
       </c>
       <c r="E29" t="n">
-        <v>-31.13323253076983</v>
+        <v>-31.13964935228265</v>
       </c>
       <c r="F29" t="n">
-        <v>1.424602687239544</v>
+        <v>1.424920472685894</v>
       </c>
       <c r="G29" t="n">
-        <v>-7.720499773627011</v>
+        <v>-7.720695333901687</v>
       </c>
     </row>
     <row r="30">
@@ -1123,13 +1123,13 @@
         <v>1.508722353123396</v>
       </c>
       <c r="E30" t="n">
-        <v>-31.02566215718053</v>
+        <v>-31.03297122244657</v>
       </c>
       <c r="F30" t="n">
-        <v>1.552601776022245</v>
+        <v>1.553085787702069</v>
       </c>
       <c r="G30" t="n">
-        <v>-7.761093197643005</v>
+        <v>-7.761234978842146</v>
       </c>
     </row>
     <row r="31">
@@ -1146,13 +1146,13 @@
         <v>1.499645910311895</v>
       </c>
       <c r="E31" t="n">
-        <v>-30.74395024799859</v>
+        <v>-30.75074352304017</v>
       </c>
       <c r="F31" t="n">
-        <v>1.459246189898504</v>
+        <v>1.459309746987774</v>
       </c>
       <c r="G31" t="n">
-        <v>-7.70382826021083</v>
+        <v>-7.703691368018557</v>
       </c>
     </row>
     <row r="32">
@@ -1169,13 +1169,13 @@
         <v>1.451615924292999</v>
       </c>
       <c r="E32" t="n">
-        <v>-30.33685731321118</v>
+        <v>-30.34416882298066</v>
       </c>
       <c r="F32" t="n">
-        <v>1.43573495587551</v>
+        <v>1.436086964369927</v>
       </c>
       <c r="G32" t="n">
-        <v>-7.698572577828897</v>
+        <v>-7.697756113682122</v>
       </c>
     </row>
     <row r="33">
@@ -1192,13 +1192,13 @@
         <v>1.359559092444087</v>
       </c>
       <c r="E33" t="n">
-        <v>-29.84176225481931</v>
+        <v>-29.84860441992955</v>
       </c>
       <c r="F33" t="n">
-        <v>1.378064230873381</v>
+        <v>1.378323348237327</v>
       </c>
       <c r="G33" t="n">
-        <v>-7.949882197808926</v>
+        <v>-7.949887086815793</v>
       </c>
     </row>
     <row r="34">
@@ -1215,13 +1215,13 @@
         <v>1.216953358123502</v>
       </c>
       <c r="E34" t="n">
-        <v>-29.26620636591518</v>
+        <v>-29.2731047546044</v>
       </c>
       <c r="F34" t="n">
-        <v>1.378548242553206</v>
+        <v>1.378919807075091</v>
       </c>
       <c r="G34" t="n">
-        <v>-7.959577098426018</v>
+        <v>-7.959464651268079</v>
       </c>
     </row>
     <row r="35">
@@ -1238,13 +1238,13 @@
         <v>1.019270275049165</v>
       </c>
       <c r="E35" t="n">
-        <v>-28.78758726066481</v>
+        <v>-28.79481076831067</v>
       </c>
       <c r="F35" t="n">
-        <v>1.394447292884413</v>
+        <v>1.39472107726896</v>
       </c>
       <c r="G35" t="n">
-        <v>-7.936012085327488</v>
+        <v>-7.935557407688865</v>
       </c>
     </row>
     <row r="36">
@@ -1261,13 +1261,13 @@
         <v>0.7623201440153018</v>
       </c>
       <c r="E36" t="n">
-        <v>-28.1573233849199</v>
+        <v>-28.16406288088594</v>
       </c>
       <c r="F36" t="n">
-        <v>1.321253971079829</v>
+        <v>1.321361529230901</v>
       </c>
       <c r="G36" t="n">
-        <v>-7.761557653295363</v>
+        <v>-7.760472293770907</v>
       </c>
     </row>
     <row r="37">
@@ -1284,13 +1284,13 @@
         <v>0.4426645192216164</v>
       </c>
       <c r="E37" t="n">
-        <v>-27.51379318904162</v>
+        <v>-27.5199215591493</v>
       </c>
       <c r="F37" t="n">
-        <v>1.410708129723772</v>
+        <v>1.410776575819909</v>
       </c>
       <c r="G37" t="n">
-        <v>-7.671947046431678</v>
+        <v>-7.671433700710652</v>
       </c>
     </row>
     <row r="38">
@@ -1307,13 +1307,13 @@
         <v>0.06096766954741239</v>
       </c>
       <c r="E38" t="n">
-        <v>-26.93205026194741</v>
+        <v>-26.93800996131818</v>
       </c>
       <c r="F38" t="n">
-        <v>1.245684591937925</v>
+        <v>1.24572370399286</v>
       </c>
       <c r="G38" t="n">
-        <v>-7.60234225566741</v>
+        <v>-7.60202447022106</v>
       </c>
     </row>
     <row r="39">
@@ -1330,13 +1330,13 @@
         <v>-0.379213195030667</v>
       </c>
       <c r="E39" t="n">
-        <v>-26.16471330067481</v>
+        <v>-26.16998853908421</v>
       </c>
       <c r="F39" t="n">
-        <v>1.329584838781052</v>
+        <v>1.329619061829121</v>
       </c>
       <c r="G39" t="n">
-        <v>-7.514961035935039</v>
+        <v>-7.514354799083542</v>
       </c>
     </row>
     <row r="40">
@@ -1353,13 +1353,13 @@
         <v>-0.876175379962664</v>
       </c>
       <c r="E40" t="n">
-        <v>-25.53146957524451</v>
+        <v>-25.53632924807023</v>
       </c>
       <c r="F40" t="n">
-        <v>1.325365625854905</v>
+        <v>1.325243400683232</v>
       </c>
       <c r="G40" t="n">
-        <v>-7.178763589724766</v>
+        <v>-7.178426248250949</v>
       </c>
     </row>
     <row r="41">
@@ -1376,13 +1376,13 @@
         <v>-1.425366338744109</v>
       </c>
       <c r="E41" t="n">
-        <v>-24.9595242179116</v>
+        <v>-24.96389010104376</v>
       </c>
       <c r="F41" t="n">
-        <v>1.380357175093964</v>
+        <v>1.380533179341173</v>
       </c>
       <c r="G41" t="n">
-        <v>-7.167846437390945</v>
+        <v>-7.166893081051896</v>
       </c>
     </row>
     <row r="42">
@@ -1399,13 +1399,13 @@
         <v>-2.015231157067687</v>
       </c>
       <c r="E42" t="n">
-        <v>-24.28090561974948</v>
+        <v>-24.28518838976489</v>
       </c>
       <c r="F42" t="n">
-        <v>1.379330483651912</v>
+        <v>1.379178924439038</v>
       </c>
       <c r="G42" t="n">
-        <v>-6.904001403804146</v>
+        <v>-6.903424500993849</v>
       </c>
     </row>
     <row r="43">
@@ -1422,13 +1422,13 @@
         <v>-2.642726177895208</v>
       </c>
       <c r="E43" t="n">
-        <v>-23.59863493345776</v>
+        <v>-23.60285903539078</v>
       </c>
       <c r="F43" t="n">
-        <v>1.332396017729528</v>
+        <v>1.332048898241977</v>
       </c>
       <c r="G43" t="n">
-        <v>-6.841598120154844</v>
+        <v>-6.841265667687893</v>
       </c>
     </row>
     <row r="44">
@@ -1445,13 +1445,13 @@
         <v>-3.302493342235634</v>
       </c>
       <c r="E44" t="n">
-        <v>-22.91155835341587</v>
+        <v>-22.91504910431884</v>
       </c>
       <c r="F44" t="n">
-        <v>1.443581811896908</v>
+        <v>1.443317805526095</v>
       </c>
       <c r="G44" t="n">
-        <v>-6.760831726713408</v>
+        <v>-6.760289046951181</v>
       </c>
     </row>
     <row r="45">
@@ -1468,13 +1468,13 @@
         <v>-3.981372365049173</v>
       </c>
       <c r="E45" t="n">
-        <v>-22.07955694281802</v>
+        <v>-22.08308680577593</v>
       </c>
       <c r="F45" t="n">
-        <v>1.488536230038191</v>
+        <v>1.488052218358366</v>
       </c>
       <c r="G45" t="n">
-        <v>-6.605884432080273</v>
+        <v>-6.60516085906397</v>
       </c>
     </row>
     <row r="46">
@@ -1491,13 +1491,13 @@
         <v>-4.675719094584308</v>
       </c>
       <c r="E46" t="n">
-        <v>-21.55803680231046</v>
+        <v>-21.56123910180829</v>
       </c>
       <c r="F46" t="n">
-        <v>1.478953776579038</v>
+        <v>1.478547989009084</v>
       </c>
       <c r="G46" t="n">
-        <v>-6.491789678827079</v>
+        <v>-6.491911903998751</v>
       </c>
     </row>
     <row r="47">
@@ -1514,13 +1514,13 @@
         <v>-5.382159326199748</v>
       </c>
       <c r="E47" t="n">
-        <v>-20.86977708260678</v>
+        <v>-20.87232425518444</v>
       </c>
       <c r="F47" t="n">
-        <v>1.560355740913172</v>
+        <v>1.560609969270251</v>
       </c>
       <c r="G47" t="n">
-        <v>-6.470009153234972</v>
+        <v>-6.46950558552768</v>
       </c>
     </row>
     <row r="48">
@@ -1537,13 +1537,13 @@
         <v>-6.091065829647205</v>
       </c>
       <c r="E48" t="n">
-        <v>-20.22664778529159</v>
+        <v>-20.2289358405053</v>
       </c>
       <c r="F48" t="n">
-        <v>1.607446655055296</v>
+        <v>1.607534657178901</v>
       </c>
       <c r="G48" t="n">
-        <v>-6.442381375430037</v>
+        <v>-6.442220038203428</v>
       </c>
     </row>
     <row r="49">
@@ -1560,13 +1560,13 @@
         <v>-6.795857888023868</v>
       </c>
       <c r="E49" t="n">
-        <v>-19.45845769232071</v>
+        <v>-19.46019817876533</v>
       </c>
       <c r="F49" t="n">
-        <v>1.751300793107402</v>
+        <v>1.751183456942596</v>
       </c>
       <c r="G49" t="n">
-        <v>-6.201504896104003</v>
+        <v>-6.201270223774392</v>
       </c>
     </row>
     <row r="50">
@@ -1583,13 +1583,13 @@
         <v>-7.495637586243298</v>
       </c>
       <c r="E50" t="n">
-        <v>-19.0580138068723</v>
+        <v>-19.05950495396671</v>
       </c>
       <c r="F50" t="n">
-        <v>1.742432134650818</v>
+        <v>1.742427245643951</v>
       </c>
       <c r="G50" t="n">
-        <v>-6.214314094095321</v>
+        <v>-6.21501322207729</v>
       </c>
     </row>
     <row r="51">
@@ -1606,13 +1606,13 @@
         <v>-8.181818297857367</v>
       </c>
       <c r="E51" t="n">
-        <v>-18.48060253986218</v>
+        <v>-18.48213768801839</v>
       </c>
       <c r="F51" t="n">
-        <v>1.719052903813231</v>
+        <v>1.719708030733398</v>
       </c>
       <c r="G51" t="n">
-        <v>-6.27375952859014</v>
+        <v>-6.274253318283698</v>
       </c>
     </row>
     <row r="52">
@@ -1629,13 +1629,13 @@
         <v>-8.840007259460942</v>
       </c>
       <c r="E52" t="n">
-        <v>-18.01583888007265</v>
+        <v>-18.01746203035246</v>
       </c>
       <c r="F52" t="n">
-        <v>1.72258765577801</v>
+        <v>1.722269870331661</v>
       </c>
       <c r="G52" t="n">
-        <v>-6.278198746825298</v>
+        <v>-6.278868540766066</v>
       </c>
     </row>
     <row r="53">
@@ -1652,13 +1652,13 @@
         <v>-9.469112857453563</v>
       </c>
       <c r="E53" t="n">
-        <v>-17.61335627876074</v>
+        <v>-17.61449541736073</v>
       </c>
       <c r="F53" t="n">
-        <v>1.809059520233135</v>
+        <v>1.808595064580778</v>
       </c>
       <c r="G53" t="n">
-        <v>-6.185874741150476</v>
+        <v>-6.186265861699829</v>
       </c>
     </row>
     <row r="54">
@@ -1675,13 +1675,13 @@
         <v>-10.06146960155995</v>
       </c>
       <c r="E54" t="n">
-        <v>-16.98467399673728</v>
+        <v>-16.98549534989092</v>
       </c>
       <c r="F54" t="n">
-        <v>1.863141714194948</v>
+        <v>1.862696814570059</v>
       </c>
       <c r="G54" t="n">
-        <v>-6.188764144208823</v>
+        <v>-6.18954638530753</v>
       </c>
     </row>
     <row r="55">
@@ -1698,13 +1698,13 @@
         <v>-10.59765823125842</v>
       </c>
       <c r="E55" t="n">
-        <v>-16.77806945554832</v>
+        <v>-16.77892014274316</v>
       </c>
       <c r="F55" t="n">
-        <v>1.852967690904898</v>
+        <v>1.852605904396746</v>
       </c>
       <c r="G55" t="n">
-        <v>-6.418273682569279</v>
+        <v>-6.419530157334076</v>
       </c>
     </row>
     <row r="56">
@@ -1721,13 +1721,13 @@
         <v>-11.07769205788199</v>
       </c>
       <c r="E56" t="n">
-        <v>-16.22583168489594</v>
+        <v>-16.22680459726246</v>
       </c>
       <c r="F56" t="n">
-        <v>1.88732274215871</v>
+        <v>1.886804507430817</v>
       </c>
       <c r="G56" t="n">
-        <v>-6.320156203757162</v>
+        <v>-6.320630437423254</v>
       </c>
     </row>
     <row r="57">
@@ -1744,13 +1744,13 @@
         <v>-11.49666896398776</v>
       </c>
       <c r="E57" t="n">
-        <v>-16.13015870951728</v>
+        <v>-16.1312196240074</v>
       </c>
       <c r="F57" t="n">
-        <v>1.927833053057967</v>
+        <v>1.927182815144667</v>
       </c>
       <c r="G57" t="n">
-        <v>-6.499866318171223</v>
+        <v>-6.501372132286232</v>
       </c>
     </row>
     <row r="58">
@@ -1767,13 +1767,13 @@
         <v>-11.83854448409222</v>
       </c>
       <c r="E58" t="n">
-        <v>-15.91586376052667</v>
+        <v>-15.91663133460477</v>
       </c>
       <c r="F58" t="n">
-        <v>1.815708569572139</v>
+        <v>1.814510762889745</v>
       </c>
       <c r="G58" t="n">
-        <v>-6.655820748218942</v>
+        <v>-6.657126113052408</v>
       </c>
     </row>
     <row r="59">
@@ -1790,13 +1790,13 @@
         <v>-12.10150994821576</v>
       </c>
       <c r="E59" t="n">
-        <v>-15.65908823086943</v>
+        <v>-15.66004158720848</v>
       </c>
       <c r="F59" t="n">
-        <v>1.870377444357982</v>
+        <v>1.869766318499618</v>
       </c>
       <c r="G59" t="n">
-        <v>-6.425142737217294</v>
+        <v>-6.425572969821583</v>
       </c>
     </row>
     <row r="60">
@@ -1813,13 +1813,13 @@
         <v>-12.28712958082474</v>
       </c>
       <c r="E60" t="n">
-        <v>-15.43579262023682</v>
+        <v>-15.43688775777501</v>
       </c>
       <c r="F60" t="n">
-        <v>1.935171452365206</v>
+        <v>1.934780331815853</v>
       </c>
       <c r="G60" t="n">
-        <v>-6.448121069491794</v>
+        <v>-6.448297073739004</v>
       </c>
     </row>
     <row r="61">
@@ -1836,13 +1836,13 @@
         <v>-12.38736964106221</v>
       </c>
       <c r="E61" t="n">
-        <v>-15.29529722990229</v>
+        <v>-15.2956639054173</v>
       </c>
       <c r="F61" t="n">
-        <v>1.881925278577635</v>
+        <v>1.881231039602534</v>
       </c>
       <c r="G61" t="n">
-        <v>-6.287776311277585</v>
+        <v>-6.287292299597761</v>
       </c>
     </row>
     <row r="62">
@@ -1859,13 +1859,13 @@
         <v>-12.39736177962232</v>
       </c>
       <c r="E62" t="n">
-        <v>-15.26634942024328</v>
+        <v>-15.2673663336716</v>
       </c>
       <c r="F62" t="n">
-        <v>1.877217164964796</v>
+        <v>1.876596261092698</v>
       </c>
       <c r="G62" t="n">
-        <v>-6.369417836948197</v>
+        <v>-6.369139163556784</v>
       </c>
     </row>
     <row r="63">
@@ -1882,13 +1882,13 @@
         <v>-12.32800270523627</v>
       </c>
       <c r="E63" t="n">
-        <v>-15.21577264420505</v>
+        <v>-15.21732245938186</v>
       </c>
       <c r="F63" t="n">
-        <v>1.863777285087647</v>
+        <v>1.863263939366621</v>
       </c>
       <c r="G63" t="n">
-        <v>-6.404276455909301</v>
+        <v>-6.403763110188275</v>
       </c>
     </row>
     <row r="64">
@@ -1905,13 +1905,13 @@
         <v>-12.17997317808845</v>
       </c>
       <c r="E64" t="n">
-        <v>-15.26452093167506</v>
+        <v>-15.26645208938749</v>
       </c>
       <c r="F64" t="n">
-        <v>1.709416671278541</v>
+        <v>1.708570873090565</v>
       </c>
       <c r="G64" t="n">
-        <v>-6.396625160162579</v>
+        <v>-6.395794028995204</v>
       </c>
     </row>
     <row r="65">
@@ -1928,13 +1928,13 @@
         <v>-11.94819266677477</v>
       </c>
       <c r="E65" t="n">
-        <v>-15.31584083675706</v>
+        <v>-15.3178013285107</v>
       </c>
       <c r="F65" t="n">
-        <v>1.701594260291478</v>
+        <v>1.701022246488049</v>
       </c>
       <c r="G65" t="n">
-        <v>-6.499132967141185</v>
+        <v>-6.498433839159216</v>
       </c>
     </row>
     <row r="66">
@@ -1951,13 +1951,13 @@
         <v>-11.64998234250278</v>
       </c>
       <c r="E66" t="n">
-        <v>-15.32433793069176</v>
+        <v>-15.3263717575484</v>
       </c>
       <c r="F66" t="n">
-        <v>1.795052515559424</v>
+        <v>1.794954735422085</v>
       </c>
       <c r="G66" t="n">
-        <v>-6.449177094975048</v>
+        <v>-6.448795752439429</v>
       </c>
     </row>
     <row r="67">
@@ -1974,13 +1974,13 @@
         <v>-11.29298322148002</v>
       </c>
       <c r="E67" t="n">
-        <v>-15.20722666020168</v>
+        <v>-15.20919204096218</v>
       </c>
       <c r="F67" t="n">
-        <v>1.617664679407149</v>
+        <v>1.617811349613156</v>
       </c>
       <c r="G67" t="n">
-        <v>-6.205851223208691</v>
+        <v>-6.204819642759772</v>
       </c>
     </row>
     <row r="68">
@@ -1997,13 +1997,13 @@
         <v>-10.87554726009174</v>
       </c>
       <c r="E68" t="n">
-        <v>-15.33994364061095</v>
+        <v>-15.34211924866673</v>
       </c>
       <c r="F68" t="n">
-        <v>1.582390494862357</v>
+        <v>1.581706033900989</v>
       </c>
       <c r="G68" t="n">
-        <v>-6.327250152721057</v>
+        <v>-6.326311463402608</v>
       </c>
     </row>
     <row r="69">
@@ -2020,13 +2020,13 @@
         <v>-10.41495874253121</v>
       </c>
       <c r="E69" t="n">
-        <v>-15.25122283299705</v>
+        <v>-15.25355488927257</v>
       </c>
       <c r="F69" t="n">
-        <v>1.544290464348489</v>
+        <v>1.543762451606862</v>
       </c>
       <c r="G69" t="n">
-        <v>-6.196449663003613</v>
+        <v>-6.195642976870572</v>
       </c>
     </row>
     <row r="70">
@@ -2043,13 +2043,13 @@
         <v>-9.922722033799177</v>
       </c>
       <c r="E70" t="n">
-        <v>-15.30273829835373</v>
+        <v>-15.30527569291766</v>
       </c>
       <c r="F70" t="n">
-        <v>1.476162153658029</v>
+        <v>1.475663474957604</v>
       </c>
       <c r="G70" t="n">
-        <v>-6.135073070796364</v>
+        <v>-6.134373942814395</v>
       </c>
     </row>
     <row r="71">
@@ -2066,13 +2066,13 @@
         <v>-9.399462252112382</v>
       </c>
       <c r="E71" t="n">
-        <v>-15.32997006660245</v>
+        <v>-15.33227278883676</v>
       </c>
       <c r="F71" t="n">
-        <v>1.368198215015947</v>
+        <v>1.367557755116381</v>
       </c>
       <c r="G71" t="n">
-        <v>-6.140455867356836</v>
+        <v>-6.139922965608343</v>
       </c>
     </row>
     <row r="72">
@@ -2089,13 +2089,13 @@
         <v>-8.852653682454918</v>
       </c>
       <c r="E72" t="n">
-        <v>-15.44807380548651</v>
+        <v>-15.45066986813284</v>
       </c>
       <c r="F72" t="n">
-        <v>1.290326113639725</v>
+        <v>1.289773655863764</v>
       </c>
       <c r="G72" t="n">
-        <v>-6.003876571522701</v>
+        <v>-6.003783680392229</v>
       </c>
     </row>
     <row r="73">
@@ -2112,13 +2112,13 @@
         <v>-8.291983786485041</v>
       </c>
       <c r="E73" t="n">
-        <v>-15.55903470533801</v>
+        <v>-15.56138142863413</v>
       </c>
       <c r="F73" t="n">
-        <v>1.221337337740688</v>
+        <v>1.221498674967297</v>
       </c>
       <c r="G73" t="n">
-        <v>-6.15358773980137</v>
+        <v>-6.153876191206519</v>
       </c>
     </row>
     <row r="74">
@@ -2135,13 +2135,13 @@
         <v>-7.715098658134548</v>
       </c>
       <c r="E74" t="n">
-        <v>-15.6717703146822</v>
+        <v>-15.6742979312324</v>
       </c>
       <c r="F74" t="n">
-        <v>1.085129606428438</v>
+        <v>1.084899823105693</v>
       </c>
       <c r="G74" t="n">
-        <v>-6.066245632123935</v>
+        <v>-6.066788311886162</v>
       </c>
     </row>
     <row r="75">
@@ -2158,13 +2158,13 @@
         <v>-7.116864474413035</v>
       </c>
       <c r="E75" t="n">
-        <v>-15.92927919536948</v>
+        <v>-15.93178236688534</v>
       </c>
       <c r="F75" t="n">
-        <v>1.030274949381652</v>
+        <v>1.02958071040655</v>
       </c>
       <c r="G75" t="n">
-        <v>-6.102952295680732</v>
+        <v>-6.103612311607765</v>
       </c>
     </row>
     <row r="76">
@@ -2181,13 +2181,13 @@
         <v>-6.50487787005311</v>
       </c>
       <c r="E76" t="n">
-        <v>-15.95348466836758</v>
+        <v>-15.95557227429975</v>
       </c>
       <c r="F76" t="n">
-        <v>0.8115505601696114</v>
+        <v>0.8109149892769124</v>
       </c>
       <c r="G76" t="n">
-        <v>-6.228462879968172</v>
+        <v>-6.228863778531259</v>
       </c>
     </row>
     <row r="77">
@@ -2204,13 +2204,13 @@
         <v>-5.874835469537738</v>
       </c>
       <c r="E77" t="n">
-        <v>-16.00682373328562</v>
+        <v>-16.00886733815599</v>
       </c>
       <c r="F77" t="n">
-        <v>0.667002183142404</v>
+        <v>0.6665279494763132</v>
       </c>
       <c r="G77" t="n">
-        <v>-6.164632006313731</v>
+        <v>-6.165003570835617</v>
       </c>
     </row>
     <row r="78">
@@ -2227,13 +2227,13 @@
         <v>-5.218958315315598</v>
       </c>
       <c r="E78" t="n">
-        <v>-16.14374037059357</v>
+        <v>-16.14580842049828</v>
       </c>
       <c r="F78" t="n">
-        <v>0.6846368309113662</v>
+        <v>0.684358157519952</v>
       </c>
       <c r="G78" t="n">
-        <v>-6.137947806834109</v>
+        <v>-6.137918472792908</v>
       </c>
     </row>
     <row r="79">
@@ -2250,13 +2250,13 @@
         <v>-4.541025940919485</v>
       </c>
       <c r="E79" t="n">
-        <v>-16.27171501434194</v>
+        <v>-16.27347505681403</v>
       </c>
       <c r="F79" t="n">
-        <v>0.3990503837873964</v>
+        <v>0.3984148128946974</v>
       </c>
       <c r="G79" t="n">
-        <v>-6.15805629207773</v>
+        <v>-6.158623416874293</v>
       </c>
     </row>
     <row r="80">
@@ -2273,13 +2273,13 @@
         <v>-3.836659558423338</v>
       </c>
       <c r="E80" t="n">
-        <v>-16.74452597943442</v>
+        <v>-16.74643758111938</v>
       </c>
       <c r="F80" t="n">
-        <v>0.3804330456381843</v>
+        <v>0.3798268087866868</v>
       </c>
       <c r="G80" t="n">
-        <v>-6.125089718774123</v>
+        <v>-6.125906182920898</v>
       </c>
     </row>
     <row r="81">
@@ -2296,13 +2296,13 @@
         <v>-3.101909809410035</v>
       </c>
       <c r="E81" t="n">
-        <v>-17.20508998232527</v>
+        <v>-17.20702602904457</v>
       </c>
       <c r="F81" t="n">
-        <v>0.2134881281536395</v>
+        <v>0.2127205540755339</v>
       </c>
       <c r="G81" t="n">
-        <v>-6.230442927749273</v>
+        <v>-6.231498953232527</v>
       </c>
     </row>
     <row r="82">
@@ -2319,13 +2319,13 @@
         <v>-2.336350650328801</v>
       </c>
       <c r="E82" t="n">
-        <v>-17.63735152446356</v>
+        <v>-17.63916534601118</v>
       </c>
       <c r="F82" t="n">
-        <v>-0.09197213188433949</v>
+        <v>-0.09266637085944142</v>
       </c>
       <c r="G82" t="n">
-        <v>-6.280657917279357</v>
+        <v>-6.281816611906816</v>
       </c>
     </row>
     <row r="83">
@@ -2342,13 +2342,13 @@
         <v>-1.54021050133261</v>
       </c>
       <c r="E83" t="n">
-        <v>-18.11372168655515</v>
+        <v>-18.11546217299977</v>
       </c>
       <c r="F83" t="n">
-        <v>-0.1033879629185859</v>
+        <v>-0.1039893107632164</v>
       </c>
       <c r="G83" t="n">
-        <v>-6.330462230232619</v>
+        <v>-6.332085380512435</v>
       </c>
     </row>
     <row r="84">
@@ -2365,13 +2365,13 @@
         <v>-0.7154325321820342</v>
       </c>
       <c r="E84" t="n">
-        <v>-18.89084399507188</v>
+        <v>-18.89208580281608</v>
       </c>
       <c r="F84" t="n">
-        <v>-0.2003711921375777</v>
+        <v>-0.2005374183710528</v>
       </c>
       <c r="G84" t="n">
-        <v>-6.361766541201476</v>
+        <v>-6.363086573055543</v>
       </c>
     </row>
     <row r="85">
@@ -2388,13 +2388,13 @@
         <v>0.1351353442662412</v>
       </c>
       <c r="E85" t="n">
-        <v>-19.57893748854209</v>
+        <v>-19.58018418529316</v>
       </c>
       <c r="F85" t="n">
-        <v>-0.3576847660943</v>
+        <v>-0.3579829955131818</v>
       </c>
       <c r="G85" t="n">
-        <v>-6.461849400774091</v>
+        <v>-6.46378544749339</v>
       </c>
     </row>
     <row r="86">
@@ -2411,13 +2411,13 @@
         <v>1.004226973751062</v>
       </c>
       <c r="E86" t="n">
-        <v>-20.23080833013533</v>
+        <v>-20.23182524356365</v>
       </c>
       <c r="F86" t="n">
-        <v>-0.5183179757136576</v>
+        <v>-0.518977991640691</v>
       </c>
       <c r="G86" t="n">
-        <v>-6.718791156664807</v>
+        <v>-6.720996098761785</v>
       </c>
     </row>
     <row r="87">
@@ -2434,13 +2434,13 @@
         <v>1.88271829117926</v>
       </c>
       <c r="E87" t="n">
-        <v>-20.98263980612951</v>
+        <v>-20.98320204191921</v>
       </c>
       <c r="F87" t="n">
-        <v>-0.6193248575841204</v>
+        <v>-0.6201559887514959</v>
       </c>
       <c r="G87" t="n">
-        <v>-7.05072538888713</v>
+        <v>-7.053551234856207</v>
       </c>
     </row>
     <row r="88">
@@ -2457,13 +2457,13 @@
         <v>2.760093217461859</v>
       </c>
       <c r="E88" t="n">
-        <v>-21.83071627130578</v>
+        <v>-21.83146917836328</v>
       </c>
       <c r="F88" t="n">
-        <v>-0.734656529574644</v>
+        <v>-0.7351649862888031</v>
       </c>
       <c r="G88" t="n">
-        <v>-7.342672433944957</v>
+        <v>-7.345542280975836</v>
       </c>
     </row>
     <row r="89">
@@ -2480,13 +2480,13 @@
         <v>3.620806604220226</v>
       </c>
       <c r="E89" t="n">
-        <v>-22.8189018952741</v>
+        <v>-22.81932723887152</v>
       </c>
       <c r="F89" t="n">
-        <v>-0.9457736241017652</v>
+        <v>-0.946883428660555</v>
       </c>
       <c r="G89" t="n">
-        <v>-7.41954228891346</v>
+        <v>-7.422338800841335</v>
       </c>
     </row>
     <row r="90">
@@ -2503,13 +2503,13 @@
         <v>4.447639326005689</v>
       </c>
       <c r="E90" t="n">
-        <v>-23.87655541781441</v>
+        <v>-23.87652119476634</v>
       </c>
       <c r="F90" t="n">
-        <v>-1.194726742771941</v>
+        <v>-1.195469871815712</v>
       </c>
       <c r="G90" t="n">
-        <v>-7.78482443697501</v>
+        <v>-7.787132048216194</v>
       </c>
     </row>
     <row r="91">
@@ -2526,13 +2526,13 @@
         <v>5.217958977477084</v>
       </c>
       <c r="E91" t="n">
-        <v>-25.08692684785654</v>
+        <v>-25.08678017765053</v>
       </c>
       <c r="F91" t="n">
-        <v>-1.12197343158538</v>
+        <v>-1.122325440079798</v>
       </c>
       <c r="G91" t="n">
-        <v>-8.155352489404761</v>
+        <v>-8.158119667291434</v>
       </c>
     </row>
     <row r="92">
@@ -2549,13 +2549,13 @@
         <v>5.910502698445531</v>
       </c>
       <c r="E92" t="n">
-        <v>-26.35522323125788</v>
+        <v>-26.35436276604931</v>
       </c>
       <c r="F92" t="n">
-        <v>-1.334816345536522</v>
+        <v>-1.334542561151975</v>
       </c>
       <c r="G92" t="n">
-        <v>-8.442405638588804</v>
+        <v>-8.446028392677189</v>
       </c>
     </row>
     <row r="93">
@@ -2572,13 +2572,13 @@
         <v>6.504421394387385</v>
       </c>
       <c r="E93" t="n">
-        <v>-27.61043418777993</v>
+        <v>-27.60990373053487</v>
       </c>
       <c r="F93" t="n">
-        <v>-1.62298907729309</v>
+        <v>-1.623272639691371</v>
       </c>
       <c r="G93" t="n">
-        <v>-8.74910770637098</v>
+        <v>-8.752794017548634</v>
       </c>
     </row>
     <row r="94">
@@ -2595,13 +2595,13 @@
         <v>6.976013478199484</v>
       </c>
       <c r="E94" t="n">
-        <v>-29.1104083840872</v>
+        <v>-29.10901501713013</v>
       </c>
       <c r="F94" t="n">
-        <v>-1.865738046249151</v>
+        <v>-1.865474039878338</v>
       </c>
       <c r="G94" t="n">
-        <v>-9.084830918915163</v>
+        <v>-9.088404782934878</v>
       </c>
     </row>
     <row r="95">
@@ -2618,13 +2618,13 @@
         <v>7.315693095126397</v>
       </c>
       <c r="E95" t="n">
-        <v>-30.74597918584836</v>
+        <v>-30.74409202919773</v>
       </c>
       <c r="F95" t="n">
-        <v>-2.126102106946707</v>
+        <v>-2.125373644923537</v>
       </c>
       <c r="G95" t="n">
-        <v>-9.356410361365421</v>
+        <v>-9.359979336378268</v>
       </c>
     </row>
     <row r="96">
@@ -2641,13 +2641,13 @@
         <v>7.508936049310361</v>
       </c>
       <c r="E96" t="n">
-        <v>-32.5826617295835</v>
+        <v>-32.58102635678652</v>
       </c>
       <c r="F96" t="n">
-        <v>-2.146719048904487</v>
+        <v>-2.145408795064154</v>
       </c>
       <c r="G96" t="n">
-        <v>-9.707817507938667</v>
+        <v>-9.711450040040784</v>
       </c>
     </row>
     <row r="97">
@@ -2664,13 +2664,13 @@
         <v>7.5578977275883</v>
       </c>
       <c r="E97" t="n">
-        <v>-34.30273901503929</v>
+        <v>-34.30073941123072</v>
       </c>
       <c r="F97" t="n">
-        <v>-2.506598844378096</v>
+        <v>-2.505298368551497</v>
       </c>
       <c r="G97" t="n">
-        <v>-10.07053292739509</v>
+        <v>-10.07422901658648</v>
       </c>
     </row>
     <row r="98">
@@ -2687,13 +2687,13 @@
         <v>7.44612886400706</v>
       </c>
       <c r="E98" t="n">
-        <v>-36.29016919650888</v>
+        <v>-36.28765624697929</v>
       </c>
       <c r="F98" t="n">
-        <v>-2.902109721897782</v>
+        <v>-2.900452348569897</v>
       </c>
       <c r="G98" t="n">
-        <v>-10.49606230707763</v>
+        <v>-10.49979750832395</v>
       </c>
     </row>
     <row r="99">
@@ -2710,13 +2710,13 @@
         <v>7.210537795491546</v>
       </c>
       <c r="E99" t="n">
-        <v>-38.32113109512149</v>
+        <v>-38.31778212541765</v>
       </c>
       <c r="F99" t="n">
-        <v>-3.178499947105085</v>
+        <v>-3.177008800010675</v>
       </c>
       <c r="G99" t="n">
-        <v>-10.82918945697548</v>
+        <v>-10.83289043517374</v>
       </c>
     </row>
     <row r="100">
@@ -2733,13 +2733,13 @@
         <v>6.815404670717444</v>
       </c>
       <c r="E100" t="n">
-        <v>-40.52218643164093</v>
+        <v>-40.51895235359846</v>
       </c>
       <c r="F100" t="n">
-        <v>-3.540345123339194</v>
+        <v>-3.539025091485127</v>
       </c>
       <c r="G100" t="n">
-        <v>-11.01871669717831</v>
+        <v>-11.02165010129846</v>
       </c>
     </row>
     <row r="101">
@@ -2756,13 +2756,13 @@
         <v>6.338435737185105</v>
       </c>
       <c r="E101" t="n">
-        <v>-42.43342633009652</v>
+        <v>-42.43057115008624</v>
       </c>
       <c r="F101" t="n">
-        <v>-3.968451009640601</v>
+        <v>-3.96737542812988</v>
       </c>
       <c r="G101" t="n">
-        <v>-11.26723958324419</v>
+        <v>-11.26974764376692</v>
       </c>
     </row>
     <row r="102">
@@ -2779,13 +2779,13 @@
         <v>5.683206153406422</v>
       </c>
       <c r="E102" t="n">
-        <v>-44.70219441172274</v>
+        <v>-44.69886010903951</v>
       </c>
       <c r="F102" t="n">
-        <v>-4.211713324317688</v>
+        <v>-4.210755078971773</v>
       </c>
       <c r="G102" t="n">
-        <v>-11.41145061879758</v>
+        <v>-11.41362622685336</v>
       </c>
     </row>
   </sheetData>

</xml_diff>